<commit_message>
Fix pre-analyser val test with MCDS 7.4
</commit_message>
<xml_diff>
--- a/tests/refout/ACDC2019-Naturalist-extrait-PreRapport.xlsx
+++ b/tests/refout/ACDC2019-Naturalist-extrait-PreRapport.xlsx
@@ -759,7 +759,7 @@
       </c>
       <c r="AI2" s="2" t="inlineStr">
         <is>
-          <t>SylvAtri-b-m-5mn-haz-cos-4brz4oei</t>
+          <t>SylvAtri-b-m-5mn-haz-cos-44bdbaqj</t>
         </is>
       </c>
     </row>
@@ -880,7 +880,7 @@
       </c>
       <c r="AI3" s="2" t="inlineStr">
         <is>
-          <t>SylvAtri-b-m-10mn-haz-cos-9ig1112l</t>
+          <t>SylvAtri-b-m-10mn-haz-cos-4mpnw3jt</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="AI4" s="2" t="inlineStr">
         <is>
-          <t>SylvAtri-ab-m-5mn-haz-cos-av6qx0cd</t>
+          <t>SylvAtri-ab-m-5mn-haz-cos-403ja14t</t>
         </is>
       </c>
     </row>
@@ -1122,7 +1122,7 @@
       </c>
       <c r="AI5" s="2" t="inlineStr">
         <is>
-          <t>SylvAtri-ab-m-10mn-haz-cos-ph1s48ue</t>
+          <t>SylvAtri-ab-m-10mn-haz-cos-vgdwfgsx</t>
         </is>
       </c>
     </row>
@@ -1243,7 +1243,7 @@
       </c>
       <c r="AI6" s="2" t="inlineStr">
         <is>
-          <t>TurdMeru-b-m-5mn-nex-cos-balhqne4</t>
+          <t>TurdMeru-b-m-5mn-nex-cos-bfydabh4</t>
         </is>
       </c>
     </row>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="AI7" s="2" t="inlineStr">
         <is>
-          <t>TurdMeru-b-m-10mn-nex-cos-hx72hpck</t>
+          <t>TurdMeru-b-m-10mn-nex-cos-dqwkobyf</t>
         </is>
       </c>
     </row>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="AI8" s="2" t="inlineStr">
         <is>
-          <t>TurdMeru-ab-m-5mn-nex-cos-x9444q0f</t>
+          <t>TurdMeru-ab-m-5mn-nex-cos-_s80wtoc</t>
         </is>
       </c>
     </row>
@@ -1606,7 +1606,7 @@
       </c>
       <c r="AI9" s="2" t="inlineStr">
         <is>
-          <t>TurdMeru-ab-m-10mn-nex-cos-6095pbq0</t>
+          <t>TurdMeru-ab-m-10mn-nex-cos-vunk_m1e</t>
         </is>
       </c>
     </row>
@@ -1727,7 +1727,7 @@
       </c>
       <c r="AI10" s="2" t="inlineStr">
         <is>
-          <t>LuscMega-b-m-5mn-nex-cos-hx9opxh4</t>
+          <t>LuscMega-b-m-5mn-nex-cos-3othwfhn</t>
         </is>
       </c>
     </row>
@@ -1848,7 +1848,7 @@
       </c>
       <c r="AI11" s="2" t="inlineStr">
         <is>
-          <t>LuscMega-b-m-10mn-nex-cos-odorvnzs</t>
+          <t>LuscMega-b-m-10mn-nex-cos-oqdu6skh</t>
         </is>
       </c>
     </row>
@@ -1969,7 +1969,7 @@
       </c>
       <c r="AI12" s="2" t="inlineStr">
         <is>
-          <t>LuscMega-ab-m-5mn-nex-cos-wjit0o_j</t>
+          <t>LuscMega-ab-m-5mn-nex-cos-_ru9tilk</t>
         </is>
       </c>
     </row>
@@ -2090,7 +2090,7 @@
       </c>
       <c r="AI13" s="2" t="inlineStr">
         <is>
-          <t>LuscMega-ab-m-10mn-nex-cos-oog7yc_8</t>
+          <t>LuscMega-ab-m-10mn-nex-cos-drd26td0</t>
         </is>
       </c>
     </row>
@@ -2105,7 +2105,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CL13"/>
+  <dimension ref="A1:CW13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2441,120 +2441,175 @@
       </c>
       <c r="BO1" s="1" t="inlineStr">
         <is>
+          <t>SansDoc #18</t>
+        </is>
+      </c>
+      <c r="BP1" s="1" t="inlineStr">
+        <is>
+          <t>SansDoc #19</t>
+        </is>
+      </c>
+      <c r="BQ1" s="1" t="inlineStr">
+        <is>
+          <t>SansDoc #20 1</t>
+        </is>
+      </c>
+      <c r="BR1" s="1" t="inlineStr">
+        <is>
+          <t>SansDoc #20 2</t>
+        </is>
+      </c>
+      <c r="BS1" s="1" t="inlineStr">
+        <is>
+          <t>SansDoc #20 3</t>
+        </is>
+      </c>
+      <c r="BT1" s="1" t="inlineStr">
+        <is>
+          <t>SansDoc #21 1</t>
+        </is>
+      </c>
+      <c r="BU1" s="1" t="inlineStr">
+        <is>
+          <t>SansDoc #21 2</t>
+        </is>
+      </c>
+      <c r="BV1" s="1" t="inlineStr">
+        <is>
+          <t>SansDoc #21 3</t>
+        </is>
+      </c>
+      <c r="BW1" s="1" t="inlineStr">
+        <is>
+          <t>SansDoc #22 1</t>
+        </is>
+      </c>
+      <c r="BX1" s="1" t="inlineStr">
+        <is>
+          <t>SansDoc #22 2</t>
+        </is>
+      </c>
+      <c r="BY1" s="1" t="inlineStr">
+        <is>
+          <t>SansDoc #22 3</t>
+        </is>
+      </c>
+      <c r="BZ1" s="1" t="inlineStr">
+        <is>
           <t>EstA(1)</t>
         </is>
       </c>
-      <c r="BP1" s="1" t="inlineStr">
+      <c r="CA1" s="1" t="inlineStr">
         <is>
           <t>EstA(2)</t>
         </is>
       </c>
-      <c r="BQ1" s="1" t="inlineStr">
+      <c r="CB1" s="1" t="inlineStr">
         <is>
           <t>DensClu</t>
         </is>
       </c>
-      <c r="BR1" s="1" t="inlineStr">
+      <c r="CC1" s="1" t="inlineStr">
         <is>
           <t>CoefVar DensClu</t>
         </is>
       </c>
-      <c r="BS1" s="1" t="inlineStr">
+      <c r="CD1" s="1" t="inlineStr">
         <is>
           <t>Min DensClu</t>
         </is>
       </c>
-      <c r="BT1" s="1" t="inlineStr">
+      <c r="CE1" s="1" t="inlineStr">
         <is>
           <t>Max DensClu</t>
         </is>
       </c>
-      <c r="BU1" s="1" t="inlineStr">
+      <c r="CF1" s="1" t="inlineStr">
         <is>
           <t>DoF DensClu</t>
         </is>
       </c>
-      <c r="BV1" s="1" t="inlineStr">
+      <c r="CG1" s="1" t="inlineStr">
         <is>
           <t>Density</t>
         </is>
       </c>
-      <c r="BW1" s="1" t="inlineStr">
+      <c r="CH1" s="1" t="inlineStr">
         <is>
           <t>Delta CoefVar Density</t>
         </is>
       </c>
-      <c r="BX1" s="1" t="inlineStr">
+      <c r="CI1" s="1" t="inlineStr">
         <is>
           <t>CoefVar Density</t>
         </is>
       </c>
-      <c r="BY1" s="1" t="inlineStr">
+      <c r="CJ1" s="1" t="inlineStr">
         <is>
           <t>Min Density</t>
         </is>
       </c>
-      <c r="BZ1" s="1" t="inlineStr">
+      <c r="CK1" s="1" t="inlineStr">
         <is>
           <t>Max Density</t>
         </is>
       </c>
-      <c r="CA1" s="1" t="inlineStr">
+      <c r="CL1" s="1" t="inlineStr">
         <is>
           <t>DoF Density</t>
         </is>
       </c>
-      <c r="CB1" s="1" t="inlineStr">
+      <c r="CM1" s="1" t="inlineStr">
         <is>
           <t>Number</t>
         </is>
       </c>
-      <c r="CC1" s="1" t="inlineStr">
+      <c r="CN1" s="1" t="inlineStr">
         <is>
           <t>CoefVar Number</t>
         </is>
       </c>
-      <c r="CD1" s="1" t="inlineStr">
+      <c r="CO1" s="1" t="inlineStr">
         <is>
           <t>Min Number</t>
         </is>
       </c>
-      <c r="CE1" s="1" t="inlineStr">
+      <c r="CP1" s="1" t="inlineStr">
         <is>
           <t>Max Number</t>
         </is>
       </c>
-      <c r="CF1" s="1" t="inlineStr">
+      <c r="CQ1" s="1" t="inlineStr">
         <is>
           <t>DoF Number</t>
         </is>
       </c>
-      <c r="CG1" s="1" t="inlineStr">
+      <c r="CR1" s="1" t="inlineStr">
         <is>
           <t>Qual Bal 1</t>
         </is>
       </c>
-      <c r="CH1" s="1" t="inlineStr">
+      <c r="CS1" s="1" t="inlineStr">
         <is>
           <t>Qual Bal 2</t>
         </is>
       </c>
-      <c r="CI1" s="1" t="inlineStr">
+      <c r="CT1" s="1" t="inlineStr">
         <is>
           <t>Qual Bal 3</t>
         </is>
       </c>
-      <c r="CJ1" s="1" t="inlineStr">
+      <c r="CU1" s="1" t="inlineStr">
         <is>
           <t>Qual Chi2+</t>
         </is>
       </c>
-      <c r="CK1" s="1" t="inlineStr">
+      <c r="CV1" s="1" t="inlineStr">
         <is>
           <t>Qual KS+</t>
         </is>
       </c>
-      <c r="CL1" s="1" t="inlineStr">
+      <c r="CW1" s="1" t="inlineStr">
         <is>
           <t>Qual DCv+</t>
         </is>
@@ -2627,14 +2682,14 @@
         <v>2</v>
       </c>
       <c r="T2" s="7" t="n">
-        <v>45368.88582466435</v>
+        <v>45386.90608821759</v>
       </c>
       <c r="U2" t="n">
-        <v>0.5392790000000001</v>
+        <v>0.574341</v>
       </c>
       <c r="V2" s="2" t="inlineStr">
         <is>
-          <t>SylvAtri-b-m-5mn-haz-cos-4brz4oei</t>
+          <t>SylvAtri-b-m-5mn-haz-cos-44bdbaqj</t>
         </is>
       </c>
       <c r="W2" t="n">
@@ -2774,75 +2829,108 @@
         <v>0</v>
       </c>
       <c r="BO2" t="n">
+        <v>1527.339</v>
+      </c>
+      <c r="BP2" t="n">
+        <v>1</v>
+      </c>
+      <c r="BQ2" t="n">
+        <v>1.264273</v>
+      </c>
+      <c r="BR2" t="n">
+        <v>1.566549</v>
+      </c>
+      <c r="BS2" t="n">
+        <v>1.322656</v>
+      </c>
+      <c r="BT2" t="n">
+        <v>4.812198</v>
+      </c>
+      <c r="BU2" t="n">
+        <v>9.740577</v>
+      </c>
+      <c r="BV2" t="n">
+        <v>12.20725</v>
+      </c>
+      <c r="BW2" t="n">
+        <v>3</v>
+      </c>
+      <c r="BX2" t="n">
+        <v>6</v>
+      </c>
+      <c r="BY2" t="n">
+        <v>11</v>
+      </c>
+      <c r="BZ2" t="n">
         <v>97.07023</v>
       </c>
-      <c r="BP2" t="n">
+      <c r="CA2" t="n">
         <v>3.818157</v>
       </c>
-      <c r="BQ2" t="n">
+      <c r="CB2" t="n">
         <v>0.2732431</v>
-      </c>
-      <c r="BR2" t="n">
-        <v>0.1593643</v>
-      </c>
-      <c r="BS2" t="n">
-        <v>0.1999974</v>
-      </c>
-      <c r="BT2" t="n">
-        <v>0.3733137</v>
-      </c>
-      <c r="BU2" t="n">
-        <v>226.7749</v>
-      </c>
-      <c r="BV2" t="n">
-        <v>0.2732431</v>
-      </c>
-      <c r="BW2" t="n">
-        <v>0</v>
-      </c>
-      <c r="BX2" s="4" t="n">
-        <v>0.1593643</v>
-      </c>
-      <c r="BY2" t="n">
-        <v>0.1999974</v>
-      </c>
-      <c r="BZ2" t="n">
-        <v>0.3733137</v>
-      </c>
-      <c r="CA2" t="n">
-        <v>226.7749</v>
-      </c>
-      <c r="CB2" t="n">
-        <v>656</v>
       </c>
       <c r="CC2" t="n">
         <v>0.1593643</v>
       </c>
       <c r="CD2" t="n">
-        <v>480</v>
+        <v>0.1999974</v>
       </c>
       <c r="CE2" t="n">
-        <v>896</v>
+        <v>0.3733137</v>
       </c>
       <c r="CF2" t="n">
         <v>226.7749</v>
       </c>
       <c r="CG2" t="n">
+        <v>0.2732431</v>
+      </c>
+      <c r="CH2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI2" s="4" t="n">
+        <v>0.1593643</v>
+      </c>
+      <c r="CJ2" t="n">
+        <v>0.1999974</v>
+      </c>
+      <c r="CK2" t="n">
+        <v>0.3733137</v>
+      </c>
+      <c r="CL2" t="n">
+        <v>226.7749</v>
+      </c>
+      <c r="CM2" t="n">
+        <v>656</v>
+      </c>
+      <c r="CN2" t="n">
+        <v>0.1593643</v>
+      </c>
+      <c r="CO2" t="n">
+        <v>480</v>
+      </c>
+      <c r="CP2" t="n">
+        <v>896</v>
+      </c>
+      <c r="CQ2" t="n">
+        <v>226.7749</v>
+      </c>
+      <c r="CR2" t="n">
         <v>0.695496362535035</v>
       </c>
-      <c r="CH2" t="n">
+      <c r="CS2" t="n">
         <v>0.6656518495714954</v>
       </c>
-      <c r="CI2" t="n">
+      <c r="CT2" t="n">
         <v>0.6773847019863569</v>
       </c>
-      <c r="CJ2" t="n">
+      <c r="CU2" t="n">
         <v>0.6291193109611052</v>
       </c>
-      <c r="CK2" t="n">
+      <c r="CV2" t="n">
         <v>0.6714278539511617</v>
       </c>
-      <c r="CL2" t="n">
+      <c r="CW2" t="n">
         <v>0.6789940363040641</v>
       </c>
     </row>
@@ -2913,14 +3001,14 @@
         <v>2</v>
       </c>
       <c r="T3" s="7" t="n">
-        <v>45368.88582528936</v>
+        <v>45386.90608967593</v>
       </c>
       <c r="U3" t="n">
-        <v>0.599803</v>
+        <v>0.5942499999999999</v>
       </c>
       <c r="V3" s="2" t="inlineStr">
         <is>
-          <t>SylvAtri-b-m-10mn-haz-cos-9ig1112l</t>
+          <t>SylvAtri-b-m-10mn-haz-cos-4mpnw3jt</t>
         </is>
       </c>
       <c r="W3" t="n">
@@ -3060,75 +3148,108 @@
         <v>0</v>
       </c>
       <c r="BO3" t="n">
+        <v>2340.707</v>
+      </c>
+      <c r="BP3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BQ3" t="n">
+        <v>1.654648</v>
+      </c>
+      <c r="BR3" t="n">
+        <v>2.34082</v>
+      </c>
+      <c r="BS3" t="n">
+        <v>1.79977</v>
+      </c>
+      <c r="BT3" t="n">
+        <v>9.927889</v>
+      </c>
+      <c r="BU3" t="n">
+        <v>23.96511</v>
+      </c>
+      <c r="BV3" t="n">
+        <v>28.82581</v>
+      </c>
+      <c r="BW3" t="n">
+        <v>6</v>
+      </c>
+      <c r="BX3" t="n">
+        <v>10</v>
+      </c>
+      <c r="BY3" t="n">
+        <v>16</v>
+      </c>
+      <c r="BZ3" t="n">
         <v>103.2911</v>
       </c>
-      <c r="BP3" t="n">
+      <c r="CA3" t="n">
         <v>3.715686</v>
       </c>
-      <c r="BQ3" t="n">
+      <c r="CB3" t="n">
         <v>0.3576427</v>
-      </c>
-      <c r="BR3" t="n">
-        <v>0.1355074</v>
-      </c>
-      <c r="BS3" t="n">
-        <v>0.2742493</v>
-      </c>
-      <c r="BT3" t="n">
-        <v>0.4663944</v>
-      </c>
-      <c r="BU3" t="n">
-        <v>288.2811</v>
-      </c>
-      <c r="BV3" t="n">
-        <v>0.3576427</v>
-      </c>
-      <c r="BW3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BX3" s="4" t="n">
-        <v>0.1355074</v>
-      </c>
-      <c r="BY3" t="n">
-        <v>0.2742493</v>
-      </c>
-      <c r="BZ3" t="n">
-        <v>0.4663944</v>
-      </c>
-      <c r="CA3" t="n">
-        <v>288.2811</v>
-      </c>
-      <c r="CB3" t="n">
-        <v>858</v>
       </c>
       <c r="CC3" t="n">
         <v>0.1355074</v>
       </c>
       <c r="CD3" t="n">
-        <v>658</v>
+        <v>0.2742493</v>
       </c>
       <c r="CE3" t="n">
-        <v>1119</v>
+        <v>0.4663944</v>
       </c>
       <c r="CF3" t="n">
         <v>288.2811</v>
       </c>
       <c r="CG3" t="n">
+        <v>0.3576427</v>
+      </c>
+      <c r="CH3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI3" s="4" t="n">
+        <v>0.1355074</v>
+      </c>
+      <c r="CJ3" t="n">
+        <v>0.2742493</v>
+      </c>
+      <c r="CK3" t="n">
+        <v>0.4663944</v>
+      </c>
+      <c r="CL3" t="n">
+        <v>288.2811</v>
+      </c>
+      <c r="CM3" t="n">
+        <v>858</v>
+      </c>
+      <c r="CN3" t="n">
+        <v>0.1355074</v>
+      </c>
+      <c r="CO3" t="n">
+        <v>658</v>
+      </c>
+      <c r="CP3" t="n">
+        <v>1119</v>
+      </c>
+      <c r="CQ3" t="n">
+        <v>288.2811</v>
+      </c>
+      <c r="CR3" t="n">
         <v>0.4666127691502999</v>
       </c>
-      <c r="CH3" t="n">
+      <c r="CS3" t="n">
         <v>0.4727497654203585</v>
       </c>
-      <c r="CI3" t="n">
+      <c r="CT3" t="n">
         <v>0.4807019138021946</v>
       </c>
-      <c r="CJ3" t="n">
+      <c r="CU3" t="n">
         <v>0.3463226928663328</v>
       </c>
-      <c r="CK3" t="n">
+      <c r="CV3" t="n">
         <v>0.4982179610788272</v>
       </c>
-      <c r="CL3" t="n">
+      <c r="CW3" t="n">
         <v>0.5080906098670958</v>
       </c>
     </row>
@@ -3199,14 +3320,14 @@
         <v>2</v>
       </c>
       <c r="T4" s="7" t="n">
-        <v>45368.88582622685</v>
+        <v>45386.90609125</v>
       </c>
       <c r="U4" t="n">
-        <v>0.616514</v>
+        <v>0.756752</v>
       </c>
       <c r="V4" s="2" t="inlineStr">
         <is>
-          <t>SylvAtri-ab-m-5mn-haz-cos-av6qx0cd</t>
+          <t>SylvAtri-ab-m-5mn-haz-cos-403ja14t</t>
         </is>
       </c>
       <c r="W4" t="n">
@@ -3346,75 +3467,108 @@
         <v>0</v>
       </c>
       <c r="BO4" t="n">
+        <v>2872.073</v>
+      </c>
+      <c r="BP4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BQ4" t="n">
+        <v>2.937908</v>
+      </c>
+      <c r="BR4" t="n">
+        <v>2.978181</v>
+      </c>
+      <c r="BS4" t="n">
+        <v>2.835873</v>
+      </c>
+      <c r="BT4" t="n">
+        <v>18.90978</v>
+      </c>
+      <c r="BU4" t="n">
+        <v>35.17652</v>
+      </c>
+      <c r="BV4" t="n">
+        <v>53.57235</v>
+      </c>
+      <c r="BW4" t="n">
+        <v>6</v>
+      </c>
+      <c r="BX4" t="n">
+        <v>11</v>
+      </c>
+      <c r="BY4" t="n">
+        <v>18</v>
+      </c>
+      <c r="BZ4" t="n">
         <v>92.10917999999999</v>
       </c>
-      <c r="BP4" t="n">
+      <c r="CA4" t="n">
         <v>3.919727</v>
       </c>
-      <c r="BQ4" t="n">
+      <c r="CB4" t="n">
         <v>0.29171</v>
-      </c>
-      <c r="BR4" t="n">
-        <v>0.1213734</v>
-      </c>
-      <c r="BS4" t="n">
-        <v>0.2299236</v>
-      </c>
-      <c r="BT4" t="n">
-        <v>0.3700999</v>
-      </c>
-      <c r="BU4" t="n">
-        <v>289.6202</v>
-      </c>
-      <c r="BV4" t="n">
-        <v>0.29171</v>
-      </c>
-      <c r="BW4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BX4" s="4" t="n">
-        <v>0.1213734</v>
-      </c>
-      <c r="BY4" t="n">
-        <v>0.2299236</v>
-      </c>
-      <c r="BZ4" t="n">
-        <v>0.3700999</v>
-      </c>
-      <c r="CA4" t="n">
-        <v>289.6202</v>
-      </c>
-      <c r="CB4" t="n">
-        <v>700</v>
       </c>
       <c r="CC4" t="n">
         <v>0.1213734</v>
       </c>
       <c r="CD4" t="n">
-        <v>552</v>
+        <v>0.2299236</v>
       </c>
       <c r="CE4" t="n">
-        <v>888</v>
+        <v>0.3700999</v>
       </c>
       <c r="CF4" t="n">
         <v>289.6202</v>
       </c>
       <c r="CG4" t="n">
+        <v>0.29171</v>
+      </c>
+      <c r="CH4" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI4" s="4" t="n">
+        <v>0.1213734</v>
+      </c>
+      <c r="CJ4" t="n">
+        <v>0.2299236</v>
+      </c>
+      <c r="CK4" t="n">
+        <v>0.3700999</v>
+      </c>
+      <c r="CL4" t="n">
+        <v>289.6202</v>
+      </c>
+      <c r="CM4" t="n">
+        <v>700</v>
+      </c>
+      <c r="CN4" t="n">
+        <v>0.1213734</v>
+      </c>
+      <c r="CO4" t="n">
+        <v>552</v>
+      </c>
+      <c r="CP4" t="n">
+        <v>888</v>
+      </c>
+      <c r="CQ4" t="n">
+        <v>289.6202</v>
+      </c>
+      <c r="CR4" t="n">
         <v>0.1796776323776616</v>
       </c>
-      <c r="CH4" t="n">
+      <c r="CS4" t="n">
         <v>0.2058511797763182</v>
       </c>
-      <c r="CI4" t="n">
+      <c r="CT4" t="n">
         <v>0.2090375699749128</v>
       </c>
-      <c r="CJ4" t="n">
+      <c r="CU4" t="n">
         <v>0.07531954883124284</v>
       </c>
-      <c r="CK4" t="n">
+      <c r="CV4" t="n">
         <v>0.2351114482088904</v>
       </c>
-      <c r="CL4" t="n">
+      <c r="CW4" t="n">
         <v>0.244043579974436</v>
       </c>
     </row>
@@ -3485,14 +3639,14 @@
         <v>2</v>
       </c>
       <c r="T5" s="7" t="n">
-        <v>45368.88582762732</v>
+        <v>45386.90609288195</v>
       </c>
       <c r="U5" t="n">
-        <v>0.668822</v>
+        <v>0.868096</v>
       </c>
       <c r="V5" s="2" t="inlineStr">
         <is>
-          <t>SylvAtri-ab-m-10mn-haz-cos-ph1s48ue</t>
+          <t>SylvAtri-ab-m-10mn-haz-cos-vgdwfgsx</t>
         </is>
       </c>
       <c r="W5" t="n">
@@ -3632,75 +3786,108 @@
         <v>0</v>
       </c>
       <c r="BO5" t="n">
+        <v>4350.866</v>
+      </c>
+      <c r="BP5" t="n">
+        <v>1</v>
+      </c>
+      <c r="BQ5" t="n">
+        <v>1.462845</v>
+      </c>
+      <c r="BR5" t="n">
+        <v>1.885604</v>
+      </c>
+      <c r="BS5" t="n">
+        <v>1.785336</v>
+      </c>
+      <c r="BT5" t="n">
+        <v>14.17539</v>
+      </c>
+      <c r="BU5" t="n">
+        <v>29.57599</v>
+      </c>
+      <c r="BV5" t="n">
+        <v>46.39332</v>
+      </c>
+      <c r="BW5" t="n">
+        <v>9</v>
+      </c>
+      <c r="BX5" t="n">
+        <v>15</v>
+      </c>
+      <c r="BY5" t="n">
+        <v>24</v>
+      </c>
+      <c r="BZ5" t="n">
         <v>99.72136</v>
       </c>
-      <c r="BP5" t="n">
+      <c r="CA5" t="n">
         <v>3.850964</v>
       </c>
-      <c r="BQ5" t="n">
+      <c r="CB5" t="n">
         <v>0.3650402</v>
-      </c>
-      <c r="BR5" t="n">
-        <v>0.1011152</v>
-      </c>
-      <c r="BS5" t="n">
-        <v>0.2993343</v>
-      </c>
-      <c r="BT5" t="n">
-        <v>0.4451689</v>
-      </c>
-      <c r="BU5" t="n">
-        <v>312.7757</v>
-      </c>
-      <c r="BV5" t="n">
-        <v>0.3650402</v>
-      </c>
-      <c r="BW5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BX5" s="4" t="n">
-        <v>0.1011152</v>
-      </c>
-      <c r="BY5" t="n">
-        <v>0.2993343</v>
-      </c>
-      <c r="BZ5" t="n">
-        <v>0.4451689</v>
-      </c>
-      <c r="CA5" t="n">
-        <v>312.7757</v>
-      </c>
-      <c r="CB5" t="n">
-        <v>876</v>
       </c>
       <c r="CC5" t="n">
         <v>0.1011152</v>
       </c>
       <c r="CD5" t="n">
-        <v>718</v>
+        <v>0.2993343</v>
       </c>
       <c r="CE5" t="n">
-        <v>1068</v>
+        <v>0.4451689</v>
       </c>
       <c r="CF5" t="n">
         <v>312.7757</v>
       </c>
       <c r="CG5" t="n">
+        <v>0.3650402</v>
+      </c>
+      <c r="CH5" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI5" s="4" t="n">
+        <v>0.1011152</v>
+      </c>
+      <c r="CJ5" t="n">
+        <v>0.2993343</v>
+      </c>
+      <c r="CK5" t="n">
+        <v>0.4451689</v>
+      </c>
+      <c r="CL5" t="n">
+        <v>312.7757</v>
+      </c>
+      <c r="CM5" t="n">
+        <v>876</v>
+      </c>
+      <c r="CN5" t="n">
+        <v>0.1011152</v>
+      </c>
+      <c r="CO5" t="n">
+        <v>718</v>
+      </c>
+      <c r="CP5" t="n">
+        <v>1068</v>
+      </c>
+      <c r="CQ5" t="n">
+        <v>312.7757</v>
+      </c>
+      <c r="CR5" t="n">
         <v>0.3688454274855517</v>
       </c>
-      <c r="CH5" t="n">
+      <c r="CS5" t="n">
         <v>0.3879872104161708</v>
       </c>
-      <c r="CI5" t="n">
+      <c r="CT5" t="n">
         <v>0.3929405784262972</v>
       </c>
-      <c r="CJ5" t="n">
+      <c r="CU5" t="n">
         <v>0.2358259125674831</v>
       </c>
-      <c r="CK5" t="n">
+      <c r="CV5" t="n">
         <v>0.4140899386931736</v>
       </c>
-      <c r="CL5" t="n">
+      <c r="CW5" t="n">
         <v>0.4309546129570214</v>
       </c>
     </row>
@@ -3771,14 +3958,14 @@
         <v>1</v>
       </c>
       <c r="T6" s="7" t="n">
-        <v>45368.88583982639</v>
+        <v>45386.90610482639</v>
       </c>
       <c r="U6" t="n">
-        <v>0.537787</v>
+        <v>0.549405</v>
       </c>
       <c r="V6" s="2" t="inlineStr">
         <is>
-          <t>TurdMeru-b-m-5mn-nex-cos-balhqne4</t>
+          <t>TurdMeru-b-m-5mn-nex-cos-bfydabh4</t>
         </is>
       </c>
       <c r="W6" t="n">
@@ -3918,73 +4105,106 @@
         <v>0</v>
       </c>
       <c r="BO6" t="n">
+        <v>1581.477</v>
+      </c>
+      <c r="BP6" t="n">
+        <v>1</v>
+      </c>
+      <c r="BQ6" t="n">
+        <v>0.5498409</v>
+      </c>
+      <c r="BR6" t="n">
+        <v>0.5520127</v>
+      </c>
+      <c r="BS6" t="n">
+        <v>1.207226</v>
+      </c>
+      <c r="BT6" t="n">
+        <v>2.267506</v>
+      </c>
+      <c r="BU6" t="n">
+        <v>2.852037</v>
+      </c>
+      <c r="BV6" t="n">
+        <v>13.09932</v>
+      </c>
+      <c r="BW6" t="n">
+        <v>4</v>
+      </c>
+      <c r="BX6" t="n">
+        <v>7</v>
+      </c>
+      <c r="BY6" t="n">
+        <v>11</v>
+      </c>
+      <c r="BZ6" t="n">
         <v>87.1977</v>
       </c>
-      <c r="BP6" s="8" t="inlineStr"/>
-      <c r="BQ6" t="n">
+      <c r="CA6" s="8" t="inlineStr"/>
+      <c r="CB6" t="n">
         <v>0.2923752</v>
-      </c>
-      <c r="BR6" t="n">
-        <v>0.1595363</v>
-      </c>
-      <c r="BS6" t="n">
-        <v>0.2139156</v>
-      </c>
-      <c r="BT6" t="n">
-        <v>0.399612</v>
-      </c>
-      <c r="BU6" t="n">
-        <v>218.1469</v>
-      </c>
-      <c r="BV6" t="n">
-        <v>0.2923752</v>
-      </c>
-      <c r="BW6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BX6" s="4" t="n">
-        <v>0.1595363</v>
-      </c>
-      <c r="BY6" t="n">
-        <v>0.2139156</v>
-      </c>
-      <c r="BZ6" t="n">
-        <v>0.399612</v>
-      </c>
-      <c r="CA6" t="n">
-        <v>218.1469</v>
-      </c>
-      <c r="CB6" t="n">
-        <v>702</v>
       </c>
       <c r="CC6" t="n">
         <v>0.1595363</v>
       </c>
       <c r="CD6" t="n">
-        <v>513</v>
+        <v>0.2139156</v>
       </c>
       <c r="CE6" t="n">
-        <v>959</v>
+        <v>0.399612</v>
       </c>
       <c r="CF6" t="n">
         <v>218.1469</v>
       </c>
       <c r="CG6" t="n">
+        <v>0.2923752</v>
+      </c>
+      <c r="CH6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI6" s="4" t="n">
+        <v>0.1595363</v>
+      </c>
+      <c r="CJ6" t="n">
+        <v>0.2139156</v>
+      </c>
+      <c r="CK6" t="n">
+        <v>0.399612</v>
+      </c>
+      <c r="CL6" t="n">
+        <v>218.1469</v>
+      </c>
+      <c r="CM6" t="n">
+        <v>702</v>
+      </c>
+      <c r="CN6" t="n">
+        <v>0.1595363</v>
+      </c>
+      <c r="CO6" t="n">
+        <v>513</v>
+      </c>
+      <c r="CP6" t="n">
+        <v>959</v>
+      </c>
+      <c r="CQ6" t="n">
+        <v>218.1469</v>
+      </c>
+      <c r="CR6" t="n">
         <v>0.6165808454832827</v>
       </c>
-      <c r="CH6" t="n">
+      <c r="CS6" t="n">
         <v>0.4788369827435124</v>
       </c>
-      <c r="CI6" t="n">
+      <c r="CT6" t="n">
         <v>0.4872760021914059</v>
       </c>
-      <c r="CJ6" t="n">
+      <c r="CU6" t="n">
         <v>0.4594219784032745</v>
       </c>
-      <c r="CK6" t="n">
+      <c r="CV6" t="n">
         <v>0.474219958583715</v>
       </c>
-      <c r="CL6" t="n">
+      <c r="CW6" t="n">
         <v>0.5065793179475074</v>
       </c>
     </row>
@@ -4055,14 +4275,14 @@
         <v>1</v>
       </c>
       <c r="T7" s="7" t="n">
-        <v>45368.88583965278</v>
+        <v>45386.90610868055</v>
       </c>
       <c r="U7" t="n">
-        <v>0.524213</v>
+        <v>0.419789</v>
       </c>
       <c r="V7" s="2" t="inlineStr">
         <is>
-          <t>TurdMeru-b-m-10mn-nex-cos-hx72hpck</t>
+          <t>TurdMeru-b-m-10mn-nex-cos-dqwkobyf</t>
         </is>
       </c>
       <c r="W7" t="n">
@@ -4202,73 +4422,106 @@
         <v>0</v>
       </c>
       <c r="BO7" t="n">
+        <v>2684.004</v>
+      </c>
+      <c r="BP7" t="n">
+        <v>1</v>
+      </c>
+      <c r="BQ7" t="n">
+        <v>2.053263</v>
+      </c>
+      <c r="BR7" t="n">
+        <v>1.781311</v>
+      </c>
+      <c r="BS7" t="n">
+        <v>1.267737</v>
+      </c>
+      <c r="BT7" t="n">
+        <v>3.047782</v>
+      </c>
+      <c r="BU7" t="n">
+        <v>6.986795</v>
+      </c>
+      <c r="BV7" t="n">
+        <v>12.02188</v>
+      </c>
+      <c r="BW7" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX7" t="n">
+        <v>9</v>
+      </c>
+      <c r="BY7" t="n">
+        <v>15</v>
+      </c>
+      <c r="BZ7" t="n">
         <v>90.15873999999999</v>
       </c>
-      <c r="BP7" s="8" t="inlineStr"/>
-      <c r="BQ7" t="n">
+      <c r="CA7" s="8" t="inlineStr"/>
+      <c r="CB7" t="n">
         <v>0.4588308</v>
-      </c>
-      <c r="BR7" t="n">
-        <v>0.1086535</v>
-      </c>
-      <c r="BS7" t="n">
-        <v>0.3707455</v>
-      </c>
-      <c r="BT7" t="n">
-        <v>0.5678443</v>
-      </c>
-      <c r="BU7" t="n">
-        <v>309.6349</v>
-      </c>
-      <c r="BV7" t="n">
-        <v>0.4588308</v>
-      </c>
-      <c r="BW7" t="n">
-        <v>0</v>
-      </c>
-      <c r="BX7" s="4" t="n">
-        <v>0.1086535</v>
-      </c>
-      <c r="BY7" t="n">
-        <v>0.3707455</v>
-      </c>
-      <c r="BZ7" t="n">
-        <v>0.5678443</v>
-      </c>
-      <c r="CA7" t="n">
-        <v>309.6349</v>
-      </c>
-      <c r="CB7" t="n">
-        <v>1101</v>
       </c>
       <c r="CC7" t="n">
         <v>0.1086535</v>
       </c>
       <c r="CD7" t="n">
-        <v>890</v>
+        <v>0.3707455</v>
       </c>
       <c r="CE7" t="n">
-        <v>1363</v>
+        <v>0.5678443</v>
       </c>
       <c r="CF7" t="n">
         <v>309.6349</v>
       </c>
       <c r="CG7" t="n">
+        <v>0.4588308</v>
+      </c>
+      <c r="CH7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI7" s="4" t="n">
+        <v>0.1086535</v>
+      </c>
+      <c r="CJ7" t="n">
+        <v>0.3707455</v>
+      </c>
+      <c r="CK7" t="n">
+        <v>0.5678443</v>
+      </c>
+      <c r="CL7" t="n">
+        <v>309.6349</v>
+      </c>
+      <c r="CM7" t="n">
+        <v>1101</v>
+      </c>
+      <c r="CN7" t="n">
+        <v>0.1086535</v>
+      </c>
+      <c r="CO7" t="n">
+        <v>890</v>
+      </c>
+      <c r="CP7" t="n">
+        <v>1363</v>
+      </c>
+      <c r="CQ7" t="n">
+        <v>309.6349</v>
+      </c>
+      <c r="CR7" t="n">
         <v>0.8281477237239776</v>
       </c>
-      <c r="CH7" t="n">
+      <c r="CS7" t="n">
         <v>0.6283725954298756</v>
       </c>
-      <c r="CI7" t="n">
+      <c r="CT7" t="n">
         <v>0.6370837699572883</v>
       </c>
-      <c r="CJ7" t="n">
+      <c r="CU7" t="n">
         <v>0.6414392368017068</v>
       </c>
-      <c r="CK7" t="n">
+      <c r="CV7" t="n">
         <v>0.644803235199809</v>
       </c>
-      <c r="CL7" t="n">
+      <c r="CW7" t="n">
         <v>0.660501585347931</v>
       </c>
     </row>
@@ -4339,14 +4592,14 @@
         <v>1</v>
       </c>
       <c r="T8" s="7" t="n">
-        <v>45368.88584394676</v>
+        <v>45386.90611225695</v>
       </c>
       <c r="U8" t="n">
-        <v>0.5017989999999999</v>
+        <v>0.7795110000000001</v>
       </c>
       <c r="V8" s="2" t="inlineStr">
         <is>
-          <t>TurdMeru-ab-m-5mn-nex-cos-x9444q0f</t>
+          <t>TurdMeru-ab-m-5mn-nex-cos-_s80wtoc</t>
         </is>
       </c>
       <c r="W8" t="n">
@@ -4486,73 +4739,106 @@
         <v>0</v>
       </c>
       <c r="BO8" t="n">
+        <v>2745.426</v>
+      </c>
+      <c r="BP8" t="n">
+        <v>1</v>
+      </c>
+      <c r="BQ8" t="n">
+        <v>0.6904538</v>
+      </c>
+      <c r="BR8" t="n">
+        <v>0.9984319</v>
+      </c>
+      <c r="BS8" t="n">
+        <v>1.003679</v>
+      </c>
+      <c r="BT8" t="n">
+        <v>2.713422</v>
+      </c>
+      <c r="BU8" t="n">
+        <v>8.238899999999999</v>
+      </c>
+      <c r="BV8" t="n">
+        <v>9.452434999999999</v>
+      </c>
+      <c r="BW8" t="n">
+        <v>6</v>
+      </c>
+      <c r="BX8" t="n">
+        <v>9</v>
+      </c>
+      <c r="BY8" t="n">
+        <v>14</v>
+      </c>
+      <c r="BZ8" t="n">
         <v>77.69714999999999</v>
       </c>
-      <c r="BP8" s="8" t="inlineStr"/>
-      <c r="BQ8" t="n">
+      <c r="CA8" s="8" t="inlineStr"/>
+      <c r="CB8" t="n">
         <v>0.32075</v>
-      </c>
-      <c r="BR8" t="n">
-        <v>0.1200648</v>
-      </c>
-      <c r="BS8" t="n">
-        <v>0.2534696</v>
-      </c>
-      <c r="BT8" t="n">
-        <v>0.4058891</v>
-      </c>
-      <c r="BU8" t="n">
-        <v>304.1691</v>
-      </c>
-      <c r="BV8" t="n">
-        <v>0.32075</v>
-      </c>
-      <c r="BW8" t="n">
-        <v>0</v>
-      </c>
-      <c r="BX8" s="4" t="n">
-        <v>0.1200648</v>
-      </c>
-      <c r="BY8" t="n">
-        <v>0.2534696</v>
-      </c>
-      <c r="BZ8" t="n">
-        <v>0.4058891</v>
-      </c>
-      <c r="CA8" t="n">
-        <v>304.1691</v>
-      </c>
-      <c r="CB8" t="n">
-        <v>770</v>
       </c>
       <c r="CC8" t="n">
         <v>0.1200648</v>
       </c>
       <c r="CD8" t="n">
-        <v>608</v>
+        <v>0.2534696</v>
       </c>
       <c r="CE8" t="n">
-        <v>974</v>
+        <v>0.4058891</v>
       </c>
       <c r="CF8" t="n">
         <v>304.1691</v>
       </c>
       <c r="CG8" t="n">
+        <v>0.32075</v>
+      </c>
+      <c r="CH8" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI8" s="4" t="n">
+        <v>0.1200648</v>
+      </c>
+      <c r="CJ8" t="n">
+        <v>0.2534696</v>
+      </c>
+      <c r="CK8" t="n">
+        <v>0.4058891</v>
+      </c>
+      <c r="CL8" t="n">
+        <v>304.1691</v>
+      </c>
+      <c r="CM8" t="n">
+        <v>770</v>
+      </c>
+      <c r="CN8" t="n">
+        <v>0.1200648</v>
+      </c>
+      <c r="CO8" t="n">
+        <v>608</v>
+      </c>
+      <c r="CP8" t="n">
+        <v>974</v>
+      </c>
+      <c r="CQ8" t="n">
+        <v>304.1691</v>
+      </c>
+      <c r="CR8" t="n">
         <v>0.9171420710519148</v>
       </c>
-      <c r="CH8" t="n">
+      <c r="CS8" t="n">
         <v>0.6852853417011571</v>
       </c>
-      <c r="CI8" t="n">
+      <c r="CT8" t="n">
         <v>0.6957899256474366</v>
       </c>
-      <c r="CJ8" t="n">
+      <c r="CU8" t="n">
         <v>0.7067639752038237</v>
       </c>
-      <c r="CK8" t="n">
+      <c r="CV8" t="n">
         <v>0.7159824689189954</v>
       </c>
-      <c r="CL8" t="n">
+      <c r="CW8" t="n">
         <v>0.7111164837963165</v>
       </c>
     </row>
@@ -4623,14 +4909,14 @@
         <v>1</v>
       </c>
       <c r="T9" s="7" t="n">
-        <v>45368.88584971065</v>
+        <v>45386.90612064815</v>
       </c>
       <c r="U9" t="n">
-        <v>0.576524</v>
+        <v>0.8188119999999999</v>
       </c>
       <c r="V9" s="2" t="inlineStr">
         <is>
-          <t>TurdMeru-ab-m-10mn-nex-cos-6095pbq0</t>
+          <t>TurdMeru-ab-m-10mn-nex-cos-vunk_m1e</t>
         </is>
       </c>
       <c r="W9" t="n">
@@ -4770,73 +5056,106 @@
         <v>0</v>
       </c>
       <c r="BO9" t="n">
+        <v>4797.853</v>
+      </c>
+      <c r="BP9" t="n">
+        <v>1</v>
+      </c>
+      <c r="BQ9" t="n">
+        <v>3.137696</v>
+      </c>
+      <c r="BR9" t="n">
+        <v>2.30542</v>
+      </c>
+      <c r="BS9" t="n">
+        <v>1.867133</v>
+      </c>
+      <c r="BT9" t="n">
+        <v>6.597888</v>
+      </c>
+      <c r="BU9" t="n">
+        <v>12.92294</v>
+      </c>
+      <c r="BV9" t="n">
+        <v>23.27799</v>
+      </c>
+      <c r="BW9" t="n">
+        <v>8</v>
+      </c>
+      <c r="BX9" t="n">
+        <v>14</v>
+      </c>
+      <c r="BY9" t="n">
+        <v>21</v>
+      </c>
+      <c r="BZ9" t="n">
         <v>82.26767</v>
       </c>
-      <c r="BP9" s="8" t="inlineStr"/>
-      <c r="BQ9" t="n">
+      <c r="CA9" s="8" t="inlineStr"/>
+      <c r="CB9" t="n">
         <v>0.495254</v>
-      </c>
-      <c r="BR9" t="n">
-        <v>0.08680069</v>
-      </c>
-      <c r="BS9" t="n">
-        <v>0.4176738</v>
-      </c>
-      <c r="BT9" t="n">
-        <v>0.5872443000000001</v>
-      </c>
-      <c r="BU9" t="n">
-        <v>366.2376</v>
-      </c>
-      <c r="BV9" t="n">
-        <v>0.495254</v>
-      </c>
-      <c r="BW9" t="n">
-        <v>0</v>
-      </c>
-      <c r="BX9" s="4" t="n">
-        <v>0.08680069</v>
-      </c>
-      <c r="BY9" t="n">
-        <v>0.4176738</v>
-      </c>
-      <c r="BZ9" t="n">
-        <v>0.5872443000000001</v>
-      </c>
-      <c r="CA9" t="n">
-        <v>366.2376</v>
-      </c>
-      <c r="CB9" t="n">
-        <v>1189</v>
       </c>
       <c r="CC9" t="n">
         <v>0.08680069</v>
       </c>
       <c r="CD9" t="n">
-        <v>1002</v>
+        <v>0.4176738</v>
       </c>
       <c r="CE9" t="n">
-        <v>1409</v>
+        <v>0.5872443000000001</v>
       </c>
       <c r="CF9" t="n">
         <v>366.2376</v>
       </c>
       <c r="CG9" t="n">
+        <v>0.495254</v>
+      </c>
+      <c r="CH9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI9" s="4" t="n">
+        <v>0.08680069</v>
+      </c>
+      <c r="CJ9" t="n">
+        <v>0.4176738</v>
+      </c>
+      <c r="CK9" t="n">
+        <v>0.5872443000000001</v>
+      </c>
+      <c r="CL9" t="n">
+        <v>366.2376</v>
+      </c>
+      <c r="CM9" t="n">
+        <v>1189</v>
+      </c>
+      <c r="CN9" t="n">
+        <v>0.08680069</v>
+      </c>
+      <c r="CO9" t="n">
+        <v>1002</v>
+      </c>
+      <c r="CP9" t="n">
+        <v>1409</v>
+      </c>
+      <c r="CQ9" t="n">
+        <v>366.2376</v>
+      </c>
+      <c r="CR9" t="n">
         <v>0.7965592486046603</v>
       </c>
-      <c r="CH9" t="n">
+      <c r="CS9" t="n">
         <v>0.6099492378990155</v>
       </c>
-      <c r="CI9" t="n">
+      <c r="CT9" t="n">
         <v>0.6163498894877982</v>
       </c>
-      <c r="CJ9" t="n">
+      <c r="CU9" t="n">
         <v>0.5748895744982946</v>
       </c>
-      <c r="CK9" t="n">
+      <c r="CV9" t="n">
         <v>0.6374939170811484</v>
       </c>
-      <c r="CL9" t="n">
+      <c r="CW9" t="n">
         <v>0.6455625569076959</v>
       </c>
     </row>
@@ -4907,14 +5226,14 @@
         <v>1</v>
       </c>
       <c r="T10" s="7" t="n">
-        <v>45368.8858625463</v>
+        <v>45386.90613228009</v>
       </c>
       <c r="U10" t="n">
-        <v>0.375461</v>
+        <v>0.557665</v>
       </c>
       <c r="V10" s="2" t="inlineStr">
         <is>
-          <t>LuscMega-b-m-5mn-nex-cos-hx9opxh4</t>
+          <t>LuscMega-b-m-5mn-nex-cos-3othwfhn</t>
         </is>
       </c>
       <c r="W10" t="n">
@@ -5054,73 +5373,106 @@
         <v>0</v>
       </c>
       <c r="BO10" t="n">
+        <v>717.264</v>
+      </c>
+      <c r="BP10" t="n">
+        <v>1</v>
+      </c>
+      <c r="BQ10" t="n">
+        <v>1.373853</v>
+      </c>
+      <c r="BR10" t="n">
+        <v>1.724357</v>
+      </c>
+      <c r="BS10" t="n">
+        <v>2.352862</v>
+      </c>
+      <c r="BT10" t="n">
+        <v>0.6097739</v>
+      </c>
+      <c r="BU10" t="n">
+        <v>1.368052</v>
+      </c>
+      <c r="BV10" t="n">
+        <v>6.376579</v>
+      </c>
+      <c r="BW10" t="n">
+        <v>1</v>
+      </c>
+      <c r="BX10" t="n">
+        <v>2</v>
+      </c>
+      <c r="BY10" t="n">
+        <v>5</v>
+      </c>
+      <c r="BZ10" t="n">
         <v>108.6992</v>
       </c>
-      <c r="BP10" s="8" t="inlineStr"/>
-      <c r="BQ10" t="n">
+      <c r="CA10" s="8" t="inlineStr"/>
+      <c r="CB10" t="n">
         <v>0.08173121999999999</v>
-      </c>
-      <c r="BR10" t="n">
-        <v>0.2167792</v>
-      </c>
-      <c r="BS10" t="n">
-        <v>0.05346113</v>
-      </c>
-      <c r="BT10" t="n">
-        <v>0.1249504</v>
-      </c>
-      <c r="BU10" t="n">
-        <v>114.9127</v>
-      </c>
-      <c r="BV10" t="n">
-        <v>0.08173121999999999</v>
-      </c>
-      <c r="BW10" t="n">
-        <v>0</v>
-      </c>
-      <c r="BX10" s="3" t="n">
-        <v>0.2167792</v>
-      </c>
-      <c r="BY10" t="n">
-        <v>0.05346113</v>
-      </c>
-      <c r="BZ10" t="n">
-        <v>0.1249504</v>
-      </c>
-      <c r="CA10" t="n">
-        <v>114.9127</v>
-      </c>
-      <c r="CB10" t="n">
-        <v>196</v>
       </c>
       <c r="CC10" t="n">
         <v>0.2167792</v>
       </c>
       <c r="CD10" t="n">
-        <v>128</v>
+        <v>0.05346113</v>
       </c>
       <c r="CE10" t="n">
-        <v>300</v>
+        <v>0.1249504</v>
       </c>
       <c r="CF10" t="n">
         <v>114.9127</v>
       </c>
       <c r="CG10" t="n">
+        <v>0.08173121999999999</v>
+      </c>
+      <c r="CH10" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI10" s="3" t="n">
+        <v>0.2167792</v>
+      </c>
+      <c r="CJ10" t="n">
+        <v>0.05346113</v>
+      </c>
+      <c r="CK10" t="n">
+        <v>0.1249504</v>
+      </c>
+      <c r="CL10" t="n">
+        <v>114.9127</v>
+      </c>
+      <c r="CM10" t="n">
+        <v>196</v>
+      </c>
+      <c r="CN10" t="n">
+        <v>0.2167792</v>
+      </c>
+      <c r="CO10" t="n">
+        <v>128</v>
+      </c>
+      <c r="CP10" t="n">
+        <v>300</v>
+      </c>
+      <c r="CQ10" t="n">
+        <v>114.9127</v>
+      </c>
+      <c r="CR10" t="n">
         <v>0.712131757907016</v>
       </c>
-      <c r="CH10" t="n">
+      <c r="CS10" t="n">
         <v>0.5315956429961963</v>
       </c>
-      <c r="CI10" t="n">
+      <c r="CT10" t="n">
         <v>0.536168314801009</v>
       </c>
-      <c r="CJ10" t="n">
+      <c r="CU10" t="n">
         <v>0.4970789335866407</v>
       </c>
-      <c r="CK10" t="n">
+      <c r="CV10" t="n">
         <v>0.563275369240733</v>
       </c>
-      <c r="CL10" t="n">
+      <c r="CW10" t="n">
         <v>0.5215934404560809</v>
       </c>
     </row>
@@ -5191,14 +5543,14 @@
         <v>1</v>
       </c>
       <c r="T11" s="7" t="n">
-        <v>45368.88585717593</v>
+        <v>45386.90612702546</v>
       </c>
       <c r="U11" t="n">
-        <v>0.547428</v>
+        <v>0.358763</v>
       </c>
       <c r="V11" s="2" t="inlineStr">
         <is>
-          <t>LuscMega-b-m-10mn-nex-cos-odorvnzs</t>
+          <t>LuscMega-b-m-10mn-nex-cos-oqdu6skh</t>
         </is>
       </c>
       <c r="W11" t="n">
@@ -5338,73 +5690,106 @@
         <v>0</v>
       </c>
       <c r="BO11" t="n">
+        <v>1054.446</v>
+      </c>
+      <c r="BP11" t="n">
+        <v>1</v>
+      </c>
+      <c r="BQ11" t="n">
+        <v>0.6924571</v>
+      </c>
+      <c r="BR11" t="n">
+        <v>1.217724</v>
+      </c>
+      <c r="BS11" t="n">
+        <v>1.076941</v>
+      </c>
+      <c r="BT11" t="n">
+        <v>0.01215697</v>
+      </c>
+      <c r="BU11" t="n">
+        <v>2.662995</v>
+      </c>
+      <c r="BV11" t="n">
+        <v>1.371374</v>
+      </c>
+      <c r="BW11" t="n">
+        <v>2</v>
+      </c>
+      <c r="BX11" t="n">
+        <v>4</v>
+      </c>
+      <c r="BY11" t="n">
+        <v>7</v>
+      </c>
+      <c r="BZ11" t="n">
         <v>112.0929</v>
       </c>
-      <c r="BP11" s="8" t="inlineStr"/>
-      <c r="BQ11" t="n">
+      <c r="CA11" s="8" t="inlineStr"/>
+      <c r="CB11" t="n">
         <v>0.1132977</v>
-      </c>
-      <c r="BR11" t="n">
-        <v>0.1864624</v>
-      </c>
-      <c r="BS11" t="n">
-        <v>0.07862413</v>
-      </c>
-      <c r="BT11" t="n">
-        <v>0.1632624</v>
-      </c>
-      <c r="BU11" t="n">
-        <v>147.4481</v>
-      </c>
-      <c r="BV11" t="n">
-        <v>0.1132977</v>
-      </c>
-      <c r="BW11" t="n">
-        <v>0</v>
-      </c>
-      <c r="BX11" s="4" t="n">
-        <v>0.1864624</v>
-      </c>
-      <c r="BY11" t="n">
-        <v>0.07862413</v>
-      </c>
-      <c r="BZ11" t="n">
-        <v>0.1632624</v>
-      </c>
-      <c r="CA11" t="n">
-        <v>147.4481</v>
-      </c>
-      <c r="CB11" t="n">
-        <v>272</v>
       </c>
       <c r="CC11" t="n">
         <v>0.1864624</v>
       </c>
       <c r="CD11" t="n">
-        <v>189</v>
+        <v>0.07862413</v>
       </c>
       <c r="CE11" t="n">
-        <v>392</v>
+        <v>0.1632624</v>
       </c>
       <c r="CF11" t="n">
         <v>147.4481</v>
       </c>
       <c r="CG11" t="n">
+        <v>0.1132977</v>
+      </c>
+      <c r="CH11" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI11" s="4" t="n">
+        <v>0.1864624</v>
+      </c>
+      <c r="CJ11" t="n">
+        <v>0.07862413</v>
+      </c>
+      <c r="CK11" t="n">
+        <v>0.1632624</v>
+      </c>
+      <c r="CL11" t="n">
+        <v>147.4481</v>
+      </c>
+      <c r="CM11" t="n">
+        <v>272</v>
+      </c>
+      <c r="CN11" t="n">
+        <v>0.1864624</v>
+      </c>
+      <c r="CO11" t="n">
+        <v>189</v>
+      </c>
+      <c r="CP11" t="n">
+        <v>392</v>
+      </c>
+      <c r="CQ11" t="n">
+        <v>147.4481</v>
+      </c>
+      <c r="CR11" t="n">
         <v>0.9395862818718695</v>
       </c>
-      <c r="CH11" t="n">
+      <c r="CS11" t="n">
         <v>0.6858354586482049</v>
       </c>
-      <c r="CI11" t="n">
+      <c r="CT11" t="n">
         <v>0.6965392329720009</v>
       </c>
-      <c r="CJ11" t="n">
+      <c r="CU11" t="n">
         <v>0.7239971702992486</v>
       </c>
-      <c r="CK11" t="n">
+      <c r="CV11" t="n">
         <v>0.7246676693514132</v>
       </c>
-      <c r="CL11" t="n">
+      <c r="CW11" t="n">
         <v>0.6804867176695002</v>
       </c>
     </row>
@@ -5475,14 +5860,14 @@
         <v>1</v>
       </c>
       <c r="T12" s="7" t="n">
-        <v>45368.88584841435</v>
+        <v>45386.90611974537</v>
       </c>
       <c r="U12" t="n">
-        <v>0.484231</v>
+        <v>0.680266</v>
       </c>
       <c r="V12" s="2" t="inlineStr">
         <is>
-          <t>LuscMega-ab-m-5mn-nex-cos-wjit0o_j</t>
+          <t>LuscMega-ab-m-5mn-nex-cos-_ru9tilk</t>
         </is>
       </c>
       <c r="W12" t="n">
@@ -5622,73 +6007,106 @@
         <v>0</v>
       </c>
       <c r="BO12" t="n">
+        <v>1333.428</v>
+      </c>
+      <c r="BP12" t="n">
+        <v>1</v>
+      </c>
+      <c r="BQ12" t="n">
+        <v>1.121317</v>
+      </c>
+      <c r="BR12" t="n">
+        <v>1.361363</v>
+      </c>
+      <c r="BS12" t="n">
+        <v>1.588817</v>
+      </c>
+      <c r="BT12" t="n">
+        <v>1.354986</v>
+      </c>
+      <c r="BU12" t="n">
+        <v>2.235081</v>
+      </c>
+      <c r="BV12" t="n">
+        <v>5.116446</v>
+      </c>
+      <c r="BW12" t="n">
+        <v>2</v>
+      </c>
+      <c r="BX12" t="n">
+        <v>5</v>
+      </c>
+      <c r="BY12" t="n">
+        <v>8</v>
+      </c>
+      <c r="BZ12" t="n">
         <v>105.3124</v>
       </c>
-      <c r="BP12" s="8" t="inlineStr"/>
-      <c r="BQ12" t="n">
+      <c r="CA12" s="8" t="inlineStr"/>
+      <c r="CB12" t="n">
         <v>0.08084502</v>
-      </c>
-      <c r="BR12" t="n">
-        <v>0.1807812</v>
-      </c>
-      <c r="BS12" t="n">
-        <v>0.05676488</v>
-      </c>
-      <c r="BT12" t="n">
-        <v>0.1151402</v>
-      </c>
-      <c r="BU12" t="n">
-        <v>200.3234</v>
-      </c>
-      <c r="BV12" t="n">
-        <v>0.08084502</v>
-      </c>
-      <c r="BW12" t="n">
-        <v>0</v>
-      </c>
-      <c r="BX12" s="4" t="n">
-        <v>0.1807812</v>
-      </c>
-      <c r="BY12" t="n">
-        <v>0.05676488</v>
-      </c>
-      <c r="BZ12" t="n">
-        <v>0.1151402</v>
-      </c>
-      <c r="CA12" t="n">
-        <v>200.3234</v>
-      </c>
-      <c r="CB12" t="n">
-        <v>194</v>
       </c>
       <c r="CC12" t="n">
         <v>0.1807812</v>
       </c>
       <c r="CD12" t="n">
-        <v>136</v>
+        <v>0.05676488</v>
       </c>
       <c r="CE12" t="n">
-        <v>276</v>
+        <v>0.1151402</v>
       </c>
       <c r="CF12" t="n">
         <v>200.3234</v>
       </c>
       <c r="CG12" t="n">
+        <v>0.08084502</v>
+      </c>
+      <c r="CH12" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI12" s="4" t="n">
+        <v>0.1807812</v>
+      </c>
+      <c r="CJ12" t="n">
+        <v>0.05676488</v>
+      </c>
+      <c r="CK12" t="n">
+        <v>0.1151402</v>
+      </c>
+      <c r="CL12" t="n">
+        <v>200.3234</v>
+      </c>
+      <c r="CM12" t="n">
+        <v>194</v>
+      </c>
+      <c r="CN12" t="n">
+        <v>0.1807812</v>
+      </c>
+      <c r="CO12" t="n">
+        <v>136</v>
+      </c>
+      <c r="CP12" t="n">
+        <v>276</v>
+      </c>
+      <c r="CQ12" t="n">
+        <v>200.3234</v>
+      </c>
+      <c r="CR12" t="n">
         <v>0.8760462080932944</v>
       </c>
-      <c r="CH12" t="n">
+      <c r="CS12" t="n">
         <v>0.6464241806373681</v>
       </c>
-      <c r="CI12" t="n">
+      <c r="CT12" t="n">
         <v>0.656980756450106</v>
       </c>
-      <c r="CJ12" t="n">
+      <c r="CU12" t="n">
         <v>0.666229198880982</v>
       </c>
-      <c r="CK12" t="n">
+      <c r="CV12" t="n">
         <v>0.6861472640215537</v>
       </c>
-      <c r="CL12" t="n">
+      <c r="CW12" t="n">
         <v>0.6494365858835733</v>
       </c>
     </row>
@@ -5759,14 +6177,14 @@
         <v>1</v>
       </c>
       <c r="T13" s="7" t="n">
-        <v>45368.88585258102</v>
+        <v>45386.9061204051</v>
       </c>
       <c r="U13" t="n">
-        <v>0.4697189999999999</v>
+        <v>0.505812</v>
       </c>
       <c r="V13" s="2" t="inlineStr">
         <is>
-          <t>LuscMega-ab-m-10mn-nex-cos-oog7yc_8</t>
+          <t>LuscMega-ab-m-10mn-nex-cos-drd26td0</t>
         </is>
       </c>
       <c r="W13" t="n">
@@ -5906,73 +6324,106 @@
         <v>0</v>
       </c>
       <c r="BO13" t="n">
+        <v>1944.133</v>
+      </c>
+      <c r="BP13" t="n">
+        <v>1</v>
+      </c>
+      <c r="BQ13" t="n">
+        <v>0.8963301</v>
+      </c>
+      <c r="BR13" t="n">
+        <v>0.9087912</v>
+      </c>
+      <c r="BS13" t="n">
+        <v>1.087616</v>
+      </c>
+      <c r="BT13" t="n">
+        <v>2.099729</v>
+      </c>
+      <c r="BU13" t="n">
+        <v>2.986194</v>
+      </c>
+      <c r="BV13" t="n">
+        <v>6.712539</v>
+      </c>
+      <c r="BW13" t="n">
+        <v>4</v>
+      </c>
+      <c r="BX13" t="n">
+        <v>7</v>
+      </c>
+      <c r="BY13" t="n">
+        <v>11</v>
+      </c>
+      <c r="BZ13" t="n">
         <v>108.5624</v>
       </c>
-      <c r="BP13" s="8" t="inlineStr"/>
-      <c r="BQ13" t="n">
+      <c r="CA13" s="8" t="inlineStr"/>
+      <c r="CB13" t="n">
         <v>0.1109432</v>
-      </c>
-      <c r="BR13" t="n">
-        <v>0.1574188</v>
-      </c>
-      <c r="BS13" t="n">
-        <v>0.08152121</v>
-      </c>
-      <c r="BT13" t="n">
-        <v>0.1509839</v>
-      </c>
-      <c r="BU13" t="n">
-        <v>247.6323</v>
-      </c>
-      <c r="BV13" t="n">
-        <v>0.1109432</v>
-      </c>
-      <c r="BW13" t="n">
-        <v>0</v>
-      </c>
-      <c r="BX13" s="4" t="n">
-        <v>0.1574188</v>
-      </c>
-      <c r="BY13" t="n">
-        <v>0.08152121</v>
-      </c>
-      <c r="BZ13" t="n">
-        <v>0.1509839</v>
-      </c>
-      <c r="CA13" t="n">
-        <v>247.6323</v>
-      </c>
-      <c r="CB13" t="n">
-        <v>266</v>
       </c>
       <c r="CC13" t="n">
         <v>0.1574188</v>
       </c>
       <c r="CD13" t="n">
-        <v>196</v>
+        <v>0.08152121</v>
       </c>
       <c r="CE13" t="n">
-        <v>362</v>
+        <v>0.1509839</v>
       </c>
       <c r="CF13" t="n">
         <v>247.6323</v>
       </c>
       <c r="CG13" t="n">
+        <v>0.1109432</v>
+      </c>
+      <c r="CH13" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI13" s="4" t="n">
+        <v>0.1574188</v>
+      </c>
+      <c r="CJ13" t="n">
+        <v>0.08152121</v>
+      </c>
+      <c r="CK13" t="n">
+        <v>0.1509839</v>
+      </c>
+      <c r="CL13" t="n">
+        <v>247.6323</v>
+      </c>
+      <c r="CM13" t="n">
+        <v>266</v>
+      </c>
+      <c r="CN13" t="n">
+        <v>0.1574188</v>
+      </c>
+      <c r="CO13" t="n">
+        <v>196</v>
+      </c>
+      <c r="CP13" t="n">
+        <v>362</v>
+      </c>
+      <c r="CQ13" t="n">
+        <v>247.6323</v>
+      </c>
+      <c r="CR13" t="n">
         <v>0.9262660551350115</v>
       </c>
-      <c r="CH13" t="n">
+      <c r="CS13" t="n">
         <v>0.6841190251436184</v>
       </c>
-      <c r="CI13" t="n">
+      <c r="CT13" t="n">
         <v>0.696187875895712</v>
       </c>
-      <c r="CJ13" t="n">
+      <c r="CU13" t="n">
         <v>0.7091441183661087</v>
       </c>
-      <c r="CK13" t="n">
+      <c r="CV13" t="n">
         <v>0.7213488936765341</v>
       </c>
-      <c r="CL13" t="n">
+      <c r="CW13" t="n">
         <v>0.6966849228483738</v>
       </c>
     </row>
@@ -7078,7 +7529,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1.0.3</t>
+          <t>1.0.3-b1</t>
         </is>
       </c>
     </row>
@@ -7090,7 +7541,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>C:/PortableApps/Distance 7/MCDS.exe</t>
+          <t>C:/PortableApps/Distance 752/MCDS.exe</t>
         </is>
       </c>
     </row>

</xml_diff>